<commit_message>
fix get wrong npc name at character config excel
</commit_message>
<xml_diff>
--- a/jyx2/Assets/Mods/JYX2/Configs/人物.xlsx
+++ b/jyx2/Assets/Mods/JYX2/Configs/人物.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\jynew\jyx2\Assets\Mods\JYX2\Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduNetdiskDownload\jynew\jyx2\Assets\Mods\JYX2\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B3F697-4844-4FFF-9698-538B8918FA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657BB898-1243-4E3E-A3D2-A7003FDDA20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8190" yWindow="1590" windowWidth="19140" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$AP$326</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="518">
   <si>
     <t>Id</t>
   </si>
@@ -1531,12 +1534,298 @@
     <t>8,13|12,11|22,10</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>欧阳克婢女</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>婢女</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>天山弟子</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>喇嘛</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>星宿弟子</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁掌弟子</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>全真弟子</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>神龙弟子</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪怪</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>千年冰蚕</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>动物</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>神雕</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>灵物</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>掌柜</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>店小</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书信</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>物</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>大夫</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>王语嫣</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>神仙姐姐</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>扫地僧</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>世外高人</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>韦小宝</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>商人</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>霍青桐</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>随从</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>软体娃娃</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1590,6 +1879,20 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1625,7 +1928,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1647,6 +1950,8 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1999,20 +2304,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP324"/>
+  <dimension ref="A1:AP337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI17" workbookViewId="0">
-      <selection activeCell="AO26" sqref="AO26"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="K332" sqref="K332"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="39" width="9" customWidth="1"/>
-    <col min="40" max="40" width="41.08984375" style="1" customWidth="1"/>
-    <col min="41" max="41" width="22.7265625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="41.06640625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="22.73046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>486</v>
       </c>
@@ -2020,7 +2325,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -2148,7 +2453,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>482</v>
       </c>
@@ -2262,7 +2567,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2665,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -2485,7 +2790,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2613,7 +2918,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2741,7 +3046,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2866,7 +3171,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -2991,7 +3296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -3116,7 +3421,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -3241,7 +3546,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -3366,7 +3671,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -3491,7 +3796,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -3619,7 +3924,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -3744,7 +4049,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -3869,7 +4174,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -3994,7 +4299,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>13</v>
       </c>
@@ -4119,7 +4424,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>14</v>
       </c>
@@ -4244,7 +4549,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>15</v>
       </c>
@@ -4369,7 +4674,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>16</v>
       </c>
@@ -4497,7 +4802,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>17</v>
       </c>
@@ -4625,7 +4930,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>18</v>
       </c>
@@ -4750,7 +5055,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -4875,7 +5180,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>20</v>
       </c>
@@ -5000,7 +5305,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>21</v>
       </c>
@@ -5125,7 +5430,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>22</v>
       </c>
@@ -5250,7 +5555,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>23</v>
       </c>
@@ -5375,7 +5680,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>24</v>
       </c>
@@ -5500,7 +5805,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>25</v>
       </c>
@@ -5628,7 +5933,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>26</v>
       </c>
@@ -5753,7 +6058,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>27</v>
       </c>
@@ -5878,7 +6183,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>28</v>
       </c>
@@ -6006,7 +6311,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>29</v>
       </c>
@@ -6134,7 +6439,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>30</v>
       </c>
@@ -6259,7 +6564,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>31</v>
       </c>
@@ -6384,7 +6689,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>32</v>
       </c>
@@ -6509,7 +6814,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>33</v>
       </c>
@@ -6634,7 +6939,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>34</v>
       </c>
@@ -6759,7 +7064,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>35</v>
       </c>
@@ -6887,7 +7192,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>36</v>
       </c>
@@ -7015,7 +7320,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>37</v>
       </c>
@@ -7143,7 +7448,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>38</v>
       </c>
@@ -7271,7 +7576,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>39</v>
       </c>
@@ -7396,7 +7701,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>40</v>
       </c>
@@ -7521,7 +7826,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>41</v>
       </c>
@@ -7646,7 +7951,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>42</v>
       </c>
@@ -7771,7 +8076,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>43</v>
       </c>
@@ -7896,7 +8201,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>44</v>
       </c>
@@ -8024,7 +8329,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>45</v>
       </c>
@@ -8152,7 +8457,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>46</v>
       </c>
@@ -8277,7 +8582,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>47</v>
       </c>
@@ -8405,7 +8710,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>48</v>
       </c>
@@ -8533,7 +8838,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>49</v>
       </c>
@@ -8661,7 +8966,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>50</v>
       </c>
@@ -8786,7 +9091,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>51</v>
       </c>
@@ -8914,7 +9219,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>52</v>
       </c>
@@ -9039,7 +9344,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>53</v>
       </c>
@@ -9167,7 +9472,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>54</v>
       </c>
@@ -9295,7 +9600,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>55</v>
       </c>
@@ -9420,7 +9725,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>56</v>
       </c>
@@ -9545,7 +9850,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>57</v>
       </c>
@@ -9670,7 +9975,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>58</v>
       </c>
@@ -9798,7 +10103,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>59</v>
       </c>
@@ -9926,7 +10231,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>60</v>
       </c>
@@ -10051,7 +10356,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>61</v>
       </c>
@@ -10179,7 +10484,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>62</v>
       </c>
@@ -10304,7 +10609,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>63</v>
       </c>
@@ -10432,7 +10737,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>64</v>
       </c>
@@ -10557,7 +10862,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>65</v>
       </c>
@@ -10682,7 +10987,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>66</v>
       </c>
@@ -10807,7 +11112,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>67</v>
       </c>
@@ -10932,7 +11237,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>68</v>
       </c>
@@ -11057,7 +11362,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>69</v>
       </c>
@@ -11182,7 +11487,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>70</v>
       </c>
@@ -11307,7 +11612,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>71</v>
       </c>
@@ -11432,7 +11737,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>72</v>
       </c>
@@ -11557,7 +11862,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>73</v>
       </c>
@@ -11682,7 +11987,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>74</v>
       </c>
@@ -11807,7 +12112,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>75</v>
       </c>
@@ -11932,7 +12237,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>76</v>
       </c>
@@ -12060,7 +12365,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>77</v>
       </c>
@@ -12185,7 +12490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:42" ht="14.5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:42" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>78</v>
       </c>
@@ -12310,7 +12615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>79</v>
       </c>
@@ -12435,7 +12740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>80</v>
       </c>
@@ -12560,7 +12865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>81</v>
       </c>
@@ -12685,7 +12990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>82</v>
       </c>
@@ -12810,7 +13115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>83</v>
       </c>
@@ -12935,7 +13240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>84</v>
       </c>
@@ -13060,7 +13365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>85</v>
       </c>
@@ -13185,7 +13490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>86</v>
       </c>
@@ -13310,7 +13615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>87</v>
       </c>
@@ -13435,7 +13740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>88</v>
       </c>
@@ -13560,7 +13865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>89</v>
       </c>
@@ -13685,7 +13990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>90</v>
       </c>
@@ -13810,7 +14115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>91</v>
       </c>
@@ -13935,7 +14240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>92</v>
       </c>
@@ -14060,7 +14365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>93</v>
       </c>
@@ -14185,7 +14490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>94</v>
       </c>
@@ -14310,7 +14615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>95</v>
       </c>
@@ -14435,7 +14740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>96</v>
       </c>
@@ -14560,7 +14865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>97</v>
       </c>
@@ -14685,7 +14990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>98</v>
       </c>
@@ -14810,7 +15115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>99</v>
       </c>
@@ -14935,7 +15240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>100</v>
       </c>
@@ -15060,7 +15365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>101</v>
       </c>
@@ -15070,8 +15375,8 @@
       <c r="C106" s="2">
         <v>3</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>348</v>
+      <c r="D106" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>348</v>
@@ -15185,7 +15490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>102</v>
       </c>
@@ -15195,8 +15500,8 @@
       <c r="C107" s="2">
         <v>4</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>348</v>
+      <c r="D107" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>348</v>
@@ -15310,7 +15615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>103</v>
       </c>
@@ -15320,8 +15625,8 @@
       <c r="C108" s="2">
         <v>6</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>348</v>
+      <c r="D108" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>348</v>
@@ -15435,7 +15740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>104</v>
       </c>
@@ -15445,8 +15750,8 @@
       <c r="C109" s="2">
         <v>7</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>348</v>
+      <c r="D109" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>348</v>
@@ -15560,7 +15865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>105</v>
       </c>
@@ -15570,8 +15875,8 @@
       <c r="C110" s="2">
         <v>6</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>348</v>
+      <c r="D110" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>348</v>
@@ -15685,7 +15990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>106</v>
       </c>
@@ -15695,8 +16000,8 @@
       <c r="C111" s="2">
         <v>5</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>348</v>
+      <c r="D111" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>348</v>
@@ -15810,7 +16115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>107</v>
       </c>
@@ -15820,8 +16125,8 @@
       <c r="C112" s="2">
         <v>6</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>348</v>
+      <c r="D112" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>348</v>
@@ -15935,7 +16240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>108</v>
       </c>
@@ -15945,8 +16250,8 @@
       <c r="C113" s="2">
         <v>7</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>348</v>
+      <c r="D113" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>348</v>
@@ -16060,7 +16365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>109</v>
       </c>
@@ -16070,8 +16375,8 @@
       <c r="C114" s="2">
         <v>6</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>348</v>
+      <c r="D114" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>348</v>
@@ -16185,7 +16490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>110</v>
       </c>
@@ -16195,8 +16500,8 @@
       <c r="C115" s="2">
         <v>8</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>348</v>
+      <c r="D115" s="11" t="s">
+        <v>497</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>348</v>
@@ -16310,7 +16615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>111</v>
       </c>
@@ -16320,8 +16625,8 @@
       <c r="C116" s="2">
         <v>9</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>356</v>
+      <c r="D116" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>356</v>
@@ -16435,7 +16740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>112</v>
       </c>
@@ -16445,8 +16750,8 @@
       <c r="C117" s="2">
         <v>9</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>356</v>
+      <c r="D117" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>356</v>
@@ -16560,7 +16865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>113</v>
       </c>
@@ -16570,8 +16875,8 @@
       <c r="C118" s="2">
         <v>9</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>356</v>
+      <c r="D118" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>356</v>
@@ -16685,7 +16990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>114</v>
       </c>
@@ -16695,8 +17000,8 @@
       <c r="C119" s="2">
         <v>8</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>356</v>
+      <c r="D119" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>356</v>
@@ -16810,7 +17115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>115</v>
       </c>
@@ -16820,8 +17125,8 @@
       <c r="C120" s="2">
         <v>9</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>356</v>
+      <c r="D120" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>356</v>
@@ -16935,7 +17240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>116</v>
       </c>
@@ -16945,8 +17250,8 @@
       <c r="C121" s="2">
         <v>9</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>356</v>
+      <c r="D121" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>356</v>
@@ -17060,7 +17365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A122" s="2">
         <v>117</v>
       </c>
@@ -17070,8 +17375,8 @@
       <c r="C122" s="2">
         <v>9</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>356</v>
+      <c r="D122" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>356</v>
@@ -17185,7 +17490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A123" s="2">
         <v>118</v>
       </c>
@@ -17195,8 +17500,8 @@
       <c r="C123" s="2">
         <v>9</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>356</v>
+      <c r="D123" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>356</v>
@@ -17310,7 +17615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A124" s="2">
         <v>119</v>
       </c>
@@ -17320,8 +17625,8 @@
       <c r="C124" s="2">
         <v>9</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>356</v>
+      <c r="D124" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>356</v>
@@ -17435,7 +17740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A125" s="2">
         <v>120</v>
       </c>
@@ -17445,8 +17750,8 @@
       <c r="C125" s="2">
         <v>9</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>356</v>
+      <c r="D125" s="11" t="s">
+        <v>498</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>356</v>
@@ -17560,7 +17865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>121</v>
       </c>
@@ -17685,7 +17990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>122</v>
       </c>
@@ -17810,7 +18115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>123</v>
       </c>
@@ -17935,7 +18240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>124</v>
       </c>
@@ -18060,7 +18365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>125</v>
       </c>
@@ -18185,7 +18490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>126</v>
       </c>
@@ -18310,7 +18615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>127</v>
       </c>
@@ -18435,7 +18740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>128</v>
       </c>
@@ -18560,7 +18865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>129</v>
       </c>
@@ -18685,7 +18990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>130</v>
       </c>
@@ -18810,7 +19115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>131</v>
       </c>
@@ -18935,7 +19240,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>132</v>
       </c>
@@ -19060,7 +19365,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>133</v>
       </c>
@@ -19185,7 +19490,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>134</v>
       </c>
@@ -19310,7 +19615,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="140" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>135</v>
       </c>
@@ -19435,7 +19740,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="141" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>136</v>
       </c>
@@ -19560,7 +19865,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="142" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>137</v>
       </c>
@@ -19685,7 +19990,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="143" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>138</v>
       </c>
@@ -19810,7 +20115,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="144" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>139</v>
       </c>
@@ -19935,7 +20240,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="145" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>140</v>
       </c>
@@ -20060,7 +20365,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="146" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>141</v>
       </c>
@@ -20185,7 +20490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="147" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A147" s="2">
         <v>142</v>
       </c>
@@ -20310,7 +20615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>143</v>
       </c>
@@ -20435,7 +20740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A149" s="2">
         <v>144</v>
       </c>
@@ -20560,7 +20865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A150" s="2">
         <v>145</v>
       </c>
@@ -20685,7 +20990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="151" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A151" s="2">
         <v>146</v>
       </c>
@@ -20810,7 +21115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="152" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A152" s="2">
         <v>147</v>
       </c>
@@ -20935,7 +21240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="153" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A153" s="2">
         <v>148</v>
       </c>
@@ -21060,7 +21365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A154" s="2">
         <v>149</v>
       </c>
@@ -21185,7 +21490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A155" s="2">
         <v>150</v>
       </c>
@@ -21310,7 +21615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A156" s="2">
         <v>151</v>
       </c>
@@ -21435,7 +21740,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="157" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A157" s="2">
         <v>152</v>
       </c>
@@ -21560,7 +21865,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="158" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A158" s="2">
         <v>153</v>
       </c>
@@ -21685,7 +21990,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="159" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A159" s="2">
         <v>154</v>
       </c>
@@ -21810,7 +22115,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="160" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A160" s="2">
         <v>155</v>
       </c>
@@ -21935,7 +22240,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="161" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A161" s="2">
         <v>156</v>
       </c>
@@ -22060,7 +22365,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="162" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A162" s="2">
         <v>157</v>
       </c>
@@ -22185,7 +22490,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="163" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A163" s="2">
         <v>158</v>
       </c>
@@ -22310,7 +22615,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="164" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A164" s="2">
         <v>159</v>
       </c>
@@ -22435,7 +22740,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="165" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A165" s="2">
         <v>160</v>
       </c>
@@ -22560,7 +22865,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="166" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A166" s="2">
         <v>161</v>
       </c>
@@ -22685,7 +22990,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="167" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A167" s="2">
         <v>162</v>
       </c>
@@ -22810,7 +23115,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="168" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A168" s="2">
         <v>163</v>
       </c>
@@ -22935,7 +23240,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="169" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A169" s="2">
         <v>164</v>
       </c>
@@ -23060,7 +23365,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="170" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A170" s="2">
         <v>165</v>
       </c>
@@ -23185,7 +23490,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="171" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A171" s="2">
         <v>166</v>
       </c>
@@ -23310,7 +23615,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="172" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A172" s="2">
         <v>167</v>
       </c>
@@ -23435,7 +23740,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="173" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A173" s="2">
         <v>168</v>
       </c>
@@ -23560,7 +23865,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="174" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A174" s="2">
         <v>169</v>
       </c>
@@ -23685,7 +23990,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="175" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A175" s="2">
         <v>170</v>
       </c>
@@ -23810,7 +24115,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="176" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A176" s="2">
         <v>171</v>
       </c>
@@ -23935,7 +24240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="177" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A177" s="2">
         <v>172</v>
       </c>
@@ -24060,7 +24365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A178" s="2">
         <v>173</v>
       </c>
@@ -24185,7 +24490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="179" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A179" s="2">
         <v>174</v>
       </c>
@@ -24310,7 +24615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="180" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A180" s="2">
         <v>175</v>
       </c>
@@ -24435,7 +24740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="181" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A181" s="2">
         <v>176</v>
       </c>
@@ -24560,7 +24865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="182" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A182" s="2">
         <v>177</v>
       </c>
@@ -24685,7 +24990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="183" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A183" s="2">
         <v>178</v>
       </c>
@@ -24810,7 +25115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="184" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A184" s="2">
         <v>179</v>
       </c>
@@ -24935,7 +25240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="185" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A185" s="2">
         <v>180</v>
       </c>
@@ -25060,7 +25365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="186" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A186" s="2">
         <v>181</v>
       </c>
@@ -25185,7 +25490,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="187" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A187" s="2">
         <v>182</v>
       </c>
@@ -25310,7 +25615,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="188" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A188" s="2">
         <v>183</v>
       </c>
@@ -25435,7 +25740,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="189" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A189" s="2">
         <v>184</v>
       </c>
@@ -25560,7 +25865,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="190" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A190" s="2">
         <v>185</v>
       </c>
@@ -25685,7 +25990,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="191" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A191" s="2">
         <v>186</v>
       </c>
@@ -25810,7 +26115,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="192" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A192" s="2">
         <v>187</v>
       </c>
@@ -25935,7 +26240,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="193" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A193" s="2">
         <v>188</v>
       </c>
@@ -26060,7 +26365,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="194" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A194" s="2">
         <v>189</v>
       </c>
@@ -26185,7 +26490,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="195" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A195" s="2">
         <v>190</v>
       </c>
@@ -26310,7 +26615,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="196" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A196" s="2">
         <v>191</v>
       </c>
@@ -26435,7 +26740,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="197" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A197" s="2">
         <v>192</v>
       </c>
@@ -26560,7 +26865,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="198" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A198" s="2">
         <v>193</v>
       </c>
@@ -26685,7 +26990,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="199" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A199" s="2">
         <v>194</v>
       </c>
@@ -26810,7 +27115,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="200" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A200" s="2">
         <v>195</v>
       </c>
@@ -26935,7 +27240,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="201" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A201" s="2">
         <v>196</v>
       </c>
@@ -27060,7 +27365,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="202" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A202" s="2">
         <v>197</v>
       </c>
@@ -27185,7 +27490,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="203" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A203" s="2">
         <v>198</v>
       </c>
@@ -27310,7 +27615,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="204" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A204" s="2">
         <v>199</v>
       </c>
@@ -27435,7 +27740,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="205" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A205" s="2">
         <v>200</v>
       </c>
@@ -27560,7 +27865,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="206" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A206" s="2">
         <v>201</v>
       </c>
@@ -27685,7 +27990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="207" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A207" s="2">
         <v>202</v>
       </c>
@@ -27810,7 +28115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="208" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A208" s="2">
         <v>203</v>
       </c>
@@ -27935,7 +28240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="209" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A209" s="2">
         <v>204</v>
       </c>
@@ -28060,7 +28365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="210" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A210" s="2">
         <v>205</v>
       </c>
@@ -28185,7 +28490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="211" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A211" s="2">
         <v>206</v>
       </c>
@@ -28310,7 +28615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="212" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A212" s="2">
         <v>207</v>
       </c>
@@ -28435,7 +28740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="213" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A213" s="2">
         <v>208</v>
       </c>
@@ -28560,7 +28865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="214" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A214" s="2">
         <v>209</v>
       </c>
@@ -28685,7 +28990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="215" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A215" s="2">
         <v>210</v>
       </c>
@@ -28810,7 +29115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="216" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A216" s="2">
         <v>211</v>
       </c>
@@ -28935,7 +29240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="217" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A217" s="2">
         <v>212</v>
       </c>
@@ -29060,7 +29365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="218" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A218" s="2">
         <v>213</v>
       </c>
@@ -29185,7 +29490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="219" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A219" s="2">
         <v>214</v>
       </c>
@@ -29310,7 +29615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="220" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A220" s="2">
         <v>215</v>
       </c>
@@ -29435,7 +29740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="221" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A221" s="2">
         <v>216</v>
       </c>
@@ -29560,7 +29865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="222" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A222" s="2">
         <v>217</v>
       </c>
@@ -29685,7 +29990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="223" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A223" s="2">
         <v>218</v>
       </c>
@@ -29810,7 +30115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="224" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A224" s="2">
         <v>219</v>
       </c>
@@ -29935,7 +30240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="225" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A225" s="2">
         <v>220</v>
       </c>
@@ -30060,7 +30365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="226" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A226" s="2">
         <v>221</v>
       </c>
@@ -30185,7 +30490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="227" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A227" s="2">
         <v>222</v>
       </c>
@@ -30310,7 +30615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="228" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A228" s="2">
         <v>223</v>
       </c>
@@ -30435,7 +30740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="229" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A229" s="2">
         <v>224</v>
       </c>
@@ -30560,7 +30865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="230" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A230" s="2">
         <v>225</v>
       </c>
@@ -30685,7 +30990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="231" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A231" s="2">
         <v>226</v>
       </c>
@@ -30810,7 +31115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="232" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A232" s="2">
         <v>227</v>
       </c>
@@ -30935,7 +31240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="233" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A233" s="2">
         <v>228</v>
       </c>
@@ -31060,7 +31365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="234" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A234" s="2">
         <v>229</v>
       </c>
@@ -31185,7 +31490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="235" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A235" s="2">
         <v>230</v>
       </c>
@@ -31310,7 +31615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="236" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A236" s="2">
         <v>231</v>
       </c>
@@ -31435,7 +31740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="237" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A237" s="2">
         <v>232</v>
       </c>
@@ -31560,7 +31865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="238" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A238" s="2">
         <v>233</v>
       </c>
@@ -31685,7 +31990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="239" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A239" s="2">
         <v>234</v>
       </c>
@@ -31810,7 +32115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="240" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A240" s="2">
         <v>235</v>
       </c>
@@ -31935,7 +32240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="241" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A241" s="2">
         <v>236</v>
       </c>
@@ -32060,7 +32365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="242" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A242" s="2">
         <v>237</v>
       </c>
@@ -32185,7 +32490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="243" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A243" s="2">
         <v>238</v>
       </c>
@@ -32310,7 +32615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="244" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A244" s="2">
         <v>239</v>
       </c>
@@ -32435,7 +32740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="245" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A245" s="2">
         <v>240</v>
       </c>
@@ -32560,7 +32865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="246" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A246" s="2">
         <v>241</v>
       </c>
@@ -32570,8 +32875,8 @@
       <c r="C246" s="2">
         <v>2</v>
       </c>
-      <c r="D246" s="2" t="s">
-        <v>429</v>
+      <c r="D246" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E246" s="2" t="s">
         <v>429</v>
@@ -32685,7 +32990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="247" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A247" s="2">
         <v>242</v>
       </c>
@@ -32695,8 +33000,8 @@
       <c r="C247" s="2">
         <v>3</v>
       </c>
-      <c r="D247" s="2" t="s">
-        <v>429</v>
+      <c r="D247" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E247" s="2" t="s">
         <v>429</v>
@@ -32810,7 +33115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="248" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A248" s="2">
         <v>243</v>
       </c>
@@ -32820,8 +33125,8 @@
       <c r="C248" s="2">
         <v>3</v>
       </c>
-      <c r="D248" s="2" t="s">
-        <v>429</v>
+      <c r="D248" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E248" s="2" t="s">
         <v>429</v>
@@ -32935,7 +33240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="249" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A249" s="2">
         <v>244</v>
       </c>
@@ -32945,8 +33250,8 @@
       <c r="C249" s="2">
         <v>3</v>
       </c>
-      <c r="D249" s="2" t="s">
-        <v>429</v>
+      <c r="D249" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E249" s="2" t="s">
         <v>429</v>
@@ -33060,7 +33365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="250" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A250" s="2">
         <v>245</v>
       </c>
@@ -33070,8 +33375,8 @@
       <c r="C250" s="2">
         <v>4</v>
       </c>
-      <c r="D250" s="2" t="s">
-        <v>429</v>
+      <c r="D250" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E250" s="2" t="s">
         <v>429</v>
@@ -33185,7 +33490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="251" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A251" s="2">
         <v>246</v>
       </c>
@@ -33195,8 +33500,8 @@
       <c r="C251" s="2">
         <v>5</v>
       </c>
-      <c r="D251" s="2" t="s">
-        <v>429</v>
+      <c r="D251" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E251" s="2" t="s">
         <v>429</v>
@@ -33310,7 +33615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="252" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A252" s="2">
         <v>247</v>
       </c>
@@ -33320,8 +33625,8 @@
       <c r="C252" s="2">
         <v>5</v>
       </c>
-      <c r="D252" s="2" t="s">
-        <v>429</v>
+      <c r="D252" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E252" s="2" t="s">
         <v>429</v>
@@ -33435,7 +33740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="253" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A253" s="2">
         <v>248</v>
       </c>
@@ -33445,8 +33750,8 @@
       <c r="C253" s="2">
         <v>5</v>
       </c>
-      <c r="D253" s="2" t="s">
-        <v>429</v>
+      <c r="D253" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E253" s="2" t="s">
         <v>429</v>
@@ -33560,7 +33865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="254" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A254" s="2">
         <v>249</v>
       </c>
@@ -33570,8 +33875,8 @@
       <c r="C254" s="2">
         <v>5</v>
       </c>
-      <c r="D254" s="2" t="s">
-        <v>429</v>
+      <c r="D254" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E254" s="2" t="s">
         <v>429</v>
@@ -33685,7 +33990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="255" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A255" s="2">
         <v>250</v>
       </c>
@@ -33695,8 +34000,8 @@
       <c r="C255" s="2">
         <v>5</v>
       </c>
-      <c r="D255" s="2" t="s">
-        <v>429</v>
+      <c r="D255" s="11" t="s">
+        <v>492</v>
       </c>
       <c r="E255" s="2" t="s">
         <v>429</v>
@@ -33810,7 +34115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="256" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A256" s="2">
         <v>251</v>
       </c>
@@ -33820,8 +34125,8 @@
       <c r="C256" s="2">
         <v>7</v>
       </c>
-      <c r="D256" s="2" t="s">
-        <v>435</v>
+      <c r="D256" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E256" s="2" t="s">
         <v>435</v>
@@ -33935,7 +34240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="257" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A257" s="2">
         <v>252</v>
       </c>
@@ -33945,8 +34250,8 @@
       <c r="C257" s="2">
         <v>7</v>
       </c>
-      <c r="D257" s="2" t="s">
-        <v>435</v>
+      <c r="D257" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E257" s="2" t="s">
         <v>435</v>
@@ -34060,7 +34365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="258" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A258" s="2">
         <v>253</v>
       </c>
@@ -34070,8 +34375,8 @@
       <c r="C258" s="2">
         <v>7</v>
       </c>
-      <c r="D258" s="2" t="s">
-        <v>435</v>
+      <c r="D258" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E258" s="2" t="s">
         <v>435</v>
@@ -34185,7 +34490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="259" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A259" s="2">
         <v>254</v>
       </c>
@@ -34195,8 +34500,8 @@
       <c r="C259" s="2">
         <v>7</v>
       </c>
-      <c r="D259" s="2" t="s">
-        <v>435</v>
+      <c r="D259" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E259" s="2" t="s">
         <v>435</v>
@@ -34310,7 +34615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="260" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A260" s="2">
         <v>255</v>
       </c>
@@ -34320,8 +34625,8 @@
       <c r="C260" s="2">
         <v>7</v>
       </c>
-      <c r="D260" s="2" t="s">
-        <v>435</v>
+      <c r="D260" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E260" s="2" t="s">
         <v>435</v>
@@ -34435,7 +34740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="261" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A261" s="2">
         <v>256</v>
       </c>
@@ -34445,8 +34750,8 @@
       <c r="C261" s="2">
         <v>7</v>
       </c>
-      <c r="D261" s="2" t="s">
-        <v>435</v>
+      <c r="D261" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E261" s="2" t="s">
         <v>435</v>
@@ -34560,7 +34865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="262" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A262" s="2">
         <v>257</v>
       </c>
@@ -34570,8 +34875,8 @@
       <c r="C262" s="2">
         <v>7</v>
       </c>
-      <c r="D262" s="2" t="s">
-        <v>435</v>
+      <c r="D262" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E262" s="2" t="s">
         <v>435</v>
@@ -34685,7 +34990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="263" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A263" s="2">
         <v>258</v>
       </c>
@@ -34695,8 +35000,8 @@
       <c r="C263" s="2">
         <v>7</v>
       </c>
-      <c r="D263" s="2" t="s">
-        <v>435</v>
+      <c r="D263" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E263" s="2" t="s">
         <v>435</v>
@@ -34810,7 +35115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="264" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A264" s="2">
         <v>259</v>
       </c>
@@ -34820,8 +35125,8 @@
       <c r="C264" s="2">
         <v>7</v>
       </c>
-      <c r="D264" s="2" t="s">
-        <v>435</v>
+      <c r="D264" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E264" s="2" t="s">
         <v>435</v>
@@ -34935,7 +35240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="265" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A265" s="2">
         <v>260</v>
       </c>
@@ -34945,8 +35250,8 @@
       <c r="C265" s="2">
         <v>7</v>
       </c>
-      <c r="D265" s="2" t="s">
-        <v>435</v>
+      <c r="D265" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="E265" s="2" t="s">
         <v>435</v>
@@ -35060,7 +35365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="266" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A266" s="2">
         <v>261</v>
       </c>
@@ -35070,8 +35375,8 @@
       <c r="C266" s="2">
         <v>5</v>
       </c>
-      <c r="D266" s="2" t="s">
-        <v>442</v>
+      <c r="D266" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E266" s="2" t="s">
         <v>442</v>
@@ -35185,7 +35490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="267" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A267" s="2">
         <v>262</v>
       </c>
@@ -35195,8 +35500,8 @@
       <c r="C267" s="2">
         <v>5</v>
       </c>
-      <c r="D267" s="2" t="s">
-        <v>442</v>
+      <c r="D267" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E267" s="2" t="s">
         <v>442</v>
@@ -35310,7 +35615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="268" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A268" s="2">
         <v>263</v>
       </c>
@@ -35320,8 +35625,8 @@
       <c r="C268" s="2">
         <v>5</v>
       </c>
-      <c r="D268" s="2" t="s">
-        <v>442</v>
+      <c r="D268" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E268" s="2" t="s">
         <v>442</v>
@@ -35435,7 +35740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="269" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A269" s="2">
         <v>264</v>
       </c>
@@ -35445,8 +35750,8 @@
       <c r="C269" s="2">
         <v>5</v>
       </c>
-      <c r="D269" s="2" t="s">
-        <v>442</v>
+      <c r="D269" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E269" s="2" t="s">
         <v>442</v>
@@ -35560,7 +35865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="270" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A270" s="2">
         <v>265</v>
       </c>
@@ -35570,8 +35875,8 @@
       <c r="C270" s="2">
         <v>5</v>
       </c>
-      <c r="D270" s="2" t="s">
-        <v>442</v>
+      <c r="D270" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E270" s="2" t="s">
         <v>442</v>
@@ -35685,7 +35990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="271" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A271" s="2">
         <v>266</v>
       </c>
@@ -35695,8 +36000,8 @@
       <c r="C271" s="2">
         <v>5</v>
       </c>
-      <c r="D271" s="2" t="s">
-        <v>442</v>
+      <c r="D271" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E271" s="2" t="s">
         <v>442</v>
@@ -35810,7 +36115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="272" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A272" s="2">
         <v>267</v>
       </c>
@@ -35820,8 +36125,8 @@
       <c r="C272" s="2">
         <v>5</v>
       </c>
-      <c r="D272" s="2" t="s">
-        <v>442</v>
+      <c r="D272" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E272" s="2" t="s">
         <v>442</v>
@@ -35935,7 +36240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="273" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A273" s="2">
         <v>268</v>
       </c>
@@ -35945,8 +36250,8 @@
       <c r="C273" s="2">
         <v>5</v>
       </c>
-      <c r="D273" s="2" t="s">
-        <v>442</v>
+      <c r="D273" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E273" s="2" t="s">
         <v>442</v>
@@ -36060,7 +36365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="274" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A274" s="2">
         <v>269</v>
       </c>
@@ -36070,8 +36375,8 @@
       <c r="C274" s="2">
         <v>5</v>
       </c>
-      <c r="D274" s="2" t="s">
-        <v>442</v>
+      <c r="D274" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E274" s="2" t="s">
         <v>442</v>
@@ -36185,7 +36490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="275" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A275" s="2">
         <v>270</v>
       </c>
@@ -36195,8 +36500,8 @@
       <c r="C275" s="2">
         <v>5</v>
       </c>
-      <c r="D275" s="2" t="s">
-        <v>442</v>
+      <c r="D275" s="11" t="s">
+        <v>494</v>
       </c>
       <c r="E275" s="2" t="s">
         <v>442</v>
@@ -36310,7 +36615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="276" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A276" s="2">
         <v>271</v>
       </c>
@@ -36435,7 +36740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="277" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A277" s="2">
         <v>272</v>
       </c>
@@ -36560,7 +36865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="278" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A278" s="2">
         <v>273</v>
       </c>
@@ -36685,7 +36990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="279" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A279" s="2">
         <v>274</v>
       </c>
@@ -36810,7 +37115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="280" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A280" s="2">
         <v>275</v>
       </c>
@@ -36935,7 +37240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="281" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A281" s="2">
         <v>276</v>
       </c>
@@ -37060,7 +37365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="282" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A282" s="2">
         <v>277</v>
       </c>
@@ -37185,7 +37490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="283" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A283" s="2">
         <v>278</v>
       </c>
@@ -37310,7 +37615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="284" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A284" s="2">
         <v>279</v>
       </c>
@@ -37435,7 +37740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="285" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A285" s="2">
         <v>280</v>
       </c>
@@ -37560,7 +37865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="286" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A286" s="2">
         <v>281</v>
       </c>
@@ -37570,8 +37875,8 @@
       <c r="C286" s="2">
         <v>5</v>
       </c>
-      <c r="D286" s="2" t="s">
-        <v>453</v>
+      <c r="D286" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E286" s="2" t="s">
         <v>453</v>
@@ -37685,7 +37990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="287" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A287" s="2">
         <v>282</v>
       </c>
@@ -37695,8 +38000,8 @@
       <c r="C287" s="2">
         <v>5</v>
       </c>
-      <c r="D287" s="2" t="s">
-        <v>453</v>
+      <c r="D287" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E287" s="2" t="s">
         <v>453</v>
@@ -37810,7 +38115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="288" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A288" s="2">
         <v>283</v>
       </c>
@@ -37820,8 +38125,8 @@
       <c r="C288" s="2">
         <v>5</v>
       </c>
-      <c r="D288" s="2" t="s">
-        <v>453</v>
+      <c r="D288" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E288" s="2" t="s">
         <v>453</v>
@@ -37935,7 +38240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="289" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A289" s="2">
         <v>284</v>
       </c>
@@ -37945,8 +38250,8 @@
       <c r="C289" s="2">
         <v>5</v>
       </c>
-      <c r="D289" s="2" t="s">
-        <v>453</v>
+      <c r="D289" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E289" s="2" t="s">
         <v>453</v>
@@ -38060,7 +38365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="290" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A290" s="2">
         <v>285</v>
       </c>
@@ -38070,8 +38375,8 @@
       <c r="C290" s="2">
         <v>5</v>
       </c>
-      <c r="D290" s="2" t="s">
-        <v>453</v>
+      <c r="D290" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E290" s="2" t="s">
         <v>453</v>
@@ -38185,7 +38490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="291" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A291" s="2">
         <v>286</v>
       </c>
@@ -38195,8 +38500,8 @@
       <c r="C291" s="2">
         <v>6</v>
       </c>
-      <c r="D291" s="2" t="s">
-        <v>453</v>
+      <c r="D291" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E291" s="2" t="s">
         <v>453</v>
@@ -38310,7 +38615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="292" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A292" s="2">
         <v>287</v>
       </c>
@@ -38320,8 +38625,8 @@
       <c r="C292" s="2">
         <v>7</v>
       </c>
-      <c r="D292" s="2" t="s">
-        <v>453</v>
+      <c r="D292" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E292" s="2" t="s">
         <v>453</v>
@@ -38435,7 +38740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="293" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A293" s="2">
         <v>288</v>
       </c>
@@ -38445,8 +38750,8 @@
       <c r="C293" s="2">
         <v>7</v>
       </c>
-      <c r="D293" s="2" t="s">
-        <v>453</v>
+      <c r="D293" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E293" s="2" t="s">
         <v>453</v>
@@ -38560,7 +38865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="294" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A294" s="2">
         <v>289</v>
       </c>
@@ -38570,8 +38875,8 @@
       <c r="C294" s="2">
         <v>7</v>
       </c>
-      <c r="D294" s="2" t="s">
-        <v>453</v>
+      <c r="D294" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E294" s="2" t="s">
         <v>453</v>
@@ -38685,7 +38990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="295" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A295" s="2">
         <v>290</v>
       </c>
@@ -38695,8 +39000,8 @@
       <c r="C295" s="2">
         <v>7</v>
       </c>
-      <c r="D295" s="2" t="s">
-        <v>453</v>
+      <c r="D295" s="11" t="s">
+        <v>495</v>
       </c>
       <c r="E295" s="2" t="s">
         <v>453</v>
@@ -38810,7 +39115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="296" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A296" s="2">
         <v>291</v>
       </c>
@@ -38820,8 +39125,8 @@
       <c r="C296" s="2">
         <v>5</v>
       </c>
-      <c r="D296" s="2" t="s">
-        <v>457</v>
+      <c r="D296" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E296" s="2" t="s">
         <v>457</v>
@@ -38935,7 +39240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="297" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A297" s="2">
         <v>292</v>
       </c>
@@ -38945,8 +39250,8 @@
       <c r="C297" s="2">
         <v>5</v>
       </c>
-      <c r="D297" s="2" t="s">
-        <v>457</v>
+      <c r="D297" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E297" s="2" t="s">
         <v>457</v>
@@ -39060,7 +39365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="298" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A298" s="2">
         <v>293</v>
       </c>
@@ -39070,8 +39375,8 @@
       <c r="C298" s="2">
         <v>5</v>
       </c>
-      <c r="D298" s="2" t="s">
-        <v>457</v>
+      <c r="D298" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E298" s="2" t="s">
         <v>457</v>
@@ -39185,7 +39490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="299" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A299" s="2">
         <v>294</v>
       </c>
@@ -39195,8 +39500,8 @@
       <c r="C299" s="2">
         <v>5</v>
       </c>
-      <c r="D299" s="2" t="s">
-        <v>457</v>
+      <c r="D299" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E299" s="2" t="s">
         <v>457</v>
@@ -39310,7 +39615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="300" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A300" s="2">
         <v>295</v>
       </c>
@@ -39320,8 +39625,8 @@
       <c r="C300" s="2">
         <v>5</v>
       </c>
-      <c r="D300" s="2" t="s">
-        <v>457</v>
+      <c r="D300" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E300" s="2" t="s">
         <v>457</v>
@@ -39435,7 +39740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="301" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A301" s="2">
         <v>296</v>
       </c>
@@ -39445,8 +39750,8 @@
       <c r="C301" s="2">
         <v>5</v>
       </c>
-      <c r="D301" s="2" t="s">
-        <v>457</v>
+      <c r="D301" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E301" s="2" t="s">
         <v>457</v>
@@ -39560,7 +39865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="302" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A302" s="2">
         <v>297</v>
       </c>
@@ -39570,8 +39875,8 @@
       <c r="C302" s="2">
         <v>5</v>
       </c>
-      <c r="D302" s="2" t="s">
-        <v>457</v>
+      <c r="D302" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E302" s="2" t="s">
         <v>457</v>
@@ -39685,7 +39990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="303" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A303" s="2">
         <v>298</v>
       </c>
@@ -39695,8 +40000,8 @@
       <c r="C303" s="2">
         <v>5</v>
       </c>
-      <c r="D303" s="2" t="s">
-        <v>457</v>
+      <c r="D303" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E303" s="2" t="s">
         <v>457</v>
@@ -39810,7 +40115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="304" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A304" s="2">
         <v>299</v>
       </c>
@@ -39820,8 +40125,8 @@
       <c r="C304" s="2">
         <v>5</v>
       </c>
-      <c r="D304" s="2" t="s">
-        <v>457</v>
+      <c r="D304" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E304" s="2" t="s">
         <v>457</v>
@@ -39935,7 +40240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="305" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:41" ht="13.9" x14ac:dyDescent="0.45">
       <c r="A305" s="2">
         <v>300</v>
       </c>
@@ -39945,8 +40250,8 @@
       <c r="C305" s="2">
         <v>5</v>
       </c>
-      <c r="D305" s="2" t="s">
-        <v>457</v>
+      <c r="D305" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="E305" s="2" t="s">
         <v>457</v>
@@ -40060,7 +40365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="306" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A306" s="2">
         <v>301</v>
       </c>
@@ -40185,7 +40490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="307" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A307" s="2">
         <v>302</v>
       </c>
@@ -40310,7 +40615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="308" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A308" s="2">
         <v>303</v>
       </c>
@@ -40435,7 +40740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="309" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A309" s="2">
         <v>304</v>
       </c>
@@ -40560,7 +40865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="310" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A310" s="2">
         <v>305</v>
       </c>
@@ -40685,7 +40990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="311" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A311" s="2">
         <v>306</v>
       </c>
@@ -40810,7 +41115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="312" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A312" s="2">
         <v>307</v>
       </c>
@@ -40935,7 +41240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="313" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A313" s="2">
         <v>308</v>
       </c>
@@ -41060,7 +41365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="314" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A314" s="2">
         <v>309</v>
       </c>
@@ -41185,7 +41490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="315" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A315" s="2">
         <v>310</v>
       </c>
@@ -41310,7 +41615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="316" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A316" s="2">
         <v>311</v>
       </c>
@@ -41435,7 +41740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="317" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A317" s="2">
         <v>312</v>
       </c>
@@ -41560,7 +41865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="318" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A318" s="2">
         <v>313</v>
       </c>
@@ -41685,7 +41990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="319" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A319" s="2">
         <v>314</v>
       </c>
@@ -41810,7 +42115,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="320" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A320" s="2">
         <v>315</v>
       </c>
@@ -41935,7 +42240,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="321" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A321" s="2">
         <v>316</v>
       </c>
@@ -42060,7 +42365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="322" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A322" s="2">
         <v>317</v>
       </c>
@@ -42185,7 +42490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="323" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A323" s="2">
         <v>318</v>
       </c>
@@ -42310,7 +42615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="324" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A324" s="2">
         <v>319</v>
       </c>
@@ -42435,7 +42740,229 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="325" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A325" s="2">
+        <v>320</v>
+      </c>
+      <c r="B325" s="2">
+        <v>89</v>
+      </c>
+      <c r="C325" s="2">
+        <v>0</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="326" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A326" s="2">
+        <v>321</v>
+      </c>
+      <c r="B326" s="2">
+        <v>103</v>
+      </c>
+      <c r="C326" s="2">
+        <v>0</v>
+      </c>
+      <c r="D326" s="12" t="s">
+        <v>499</v>
+      </c>
+      <c r="E326" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="327" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A327" s="2">
+        <v>322</v>
+      </c>
+      <c r="B327" s="2">
+        <v>104</v>
+      </c>
+      <c r="C327" s="2">
+        <v>0</v>
+      </c>
+      <c r="D327" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E327" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="328" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A328" s="2">
+        <v>323</v>
+      </c>
+      <c r="B328" s="2">
+        <v>105</v>
+      </c>
+      <c r="C328" s="2">
+        <v>0</v>
+      </c>
+      <c r="D328" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="E328" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="329" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A329" s="2">
+        <v>324</v>
+      </c>
+      <c r="B329" s="2">
+        <v>106</v>
+      </c>
+      <c r="C329" s="2">
+        <v>0</v>
+      </c>
+      <c r="D329" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="E329" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="330" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A330" s="2">
+        <v>325</v>
+      </c>
+      <c r="B330" s="2">
+        <v>107</v>
+      </c>
+      <c r="C330" s="2">
+        <v>0</v>
+      </c>
+      <c r="D330" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E330" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="331" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A331" s="2">
+        <v>326</v>
+      </c>
+      <c r="B331" s="2">
+        <v>108</v>
+      </c>
+      <c r="C331" s="2">
+        <v>0</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="E331" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="332" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A332" s="2">
+        <v>327</v>
+      </c>
+      <c r="B332" s="2">
+        <v>109</v>
+      </c>
+      <c r="C332" s="2">
+        <v>0</v>
+      </c>
+      <c r="D332" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="E332" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="333" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A333" s="2">
+        <v>328</v>
+      </c>
+      <c r="B333" s="2">
+        <v>110</v>
+      </c>
+      <c r="C333" s="2">
+        <v>0</v>
+      </c>
+      <c r="D333" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E333" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="334" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A334" s="2">
+        <v>329</v>
+      </c>
+      <c r="B334" s="2">
+        <v>111</v>
+      </c>
+      <c r="C334" s="2">
+        <v>0</v>
+      </c>
+      <c r="D334" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E334" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="335" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A335" s="2">
+        <v>330</v>
+      </c>
+      <c r="B335" s="2">
+        <v>112</v>
+      </c>
+      <c r="C335" s="2">
+        <v>0</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E335" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="336" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A336" s="2">
+        <v>331</v>
+      </c>
+      <c r="B336" s="2">
+        <v>113</v>
+      </c>
+      <c r="C336" s="2">
+        <v>0</v>
+      </c>
+      <c r="D336" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="E336" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A337" s="2">
+        <v>332</v>
+      </c>
+      <c r="B337" s="2">
+        <v>114</v>
+      </c>
+      <c r="C337" s="2">
+        <v>0</v>
+      </c>
+      <c r="D337" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="E337" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A4:AP326" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>